<commit_message>
Uploading the correct pupae and fly data from excel.
</commit_message>
<xml_diff>
--- a/data/fitness_experiment/pupae_data.xlsx
+++ b/data/fitness_experiment/pupae_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katherinemillar/Documents/microbial-impacts-on-dietary-choice-in-drosophila-melanogaster_9/data/fitness_experiment/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6BC698EE-AF05-344E-8BC1-84057EA439D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCFA2F9-A553-3B48-A636-DC28469569F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{3D6DB07D-0F87-E944-B2F3-9A7591BBA46C}"/>
   </bookViews>
@@ -47,13 +47,13 @@
     <t>conditioned</t>
   </si>
   <si>
-    <t>time (hours)</t>
-  </si>
-  <si>
     <t>pupae</t>
   </si>
   <si>
     <t>unconditioned</t>
+  </si>
+  <si>
+    <t>time_hours</t>
   </si>
 </sst>
 </file>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77C8FBC1-AEEF-6C4A-9797-D4DB6B28D6A6}">
   <dimension ref="A1:D661"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D662" sqref="D662"/>
+    <sheetView tabSelected="1" zoomScale="140" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -444,10 +444,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -469,7 +469,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>202</v>
@@ -497,7 +497,7 @@
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5">
         <v>209</v>
@@ -525,7 +525,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7">
         <v>226</v>
@@ -553,7 +553,7 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9">
         <v>231</v>
@@ -581,7 +581,7 @@
         <v>1</v>
       </c>
       <c r="B11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C11">
         <v>250</v>
@@ -609,7 +609,7 @@
         <v>1</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <v>255</v>
@@ -637,7 +637,7 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
         <v>274</v>
@@ -665,7 +665,7 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
         <v>279</v>
@@ -693,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19">
         <v>298</v>
@@ -721,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21">
         <v>303</v>
@@ -749,7 +749,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23">
         <v>320</v>
@@ -777,7 +777,7 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25">
         <v>202</v>
@@ -805,7 +805,7 @@
         <v>2</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27">
         <v>209</v>
@@ -833,7 +833,7 @@
         <v>2</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29">
         <v>226</v>
@@ -861,7 +861,7 @@
         <v>2</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31">
         <v>231</v>
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33">
         <v>250</v>
@@ -917,7 +917,7 @@
         <v>2</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35">
         <v>255</v>
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="B37" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37">
         <v>274</v>
@@ -973,7 +973,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39">
         <v>279</v>
@@ -1001,7 +1001,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41">
         <v>298</v>
@@ -1029,7 +1029,7 @@
         <v>2</v>
       </c>
       <c r="B43" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43">
         <v>303</v>
@@ -1057,7 +1057,7 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45">
         <v>320</v>
@@ -1085,7 +1085,7 @@
         <v>3</v>
       </c>
       <c r="B47" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47">
         <v>202</v>
@@ -1113,7 +1113,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C49">
         <v>209</v>
@@ -1141,7 +1141,7 @@
         <v>3</v>
       </c>
       <c r="B51" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51">
         <v>226</v>
@@ -1169,7 +1169,7 @@
         <v>3</v>
       </c>
       <c r="B53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C53">
         <v>231</v>
@@ -1197,7 +1197,7 @@
         <v>3</v>
       </c>
       <c r="B55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C55">
         <v>250</v>
@@ -1225,7 +1225,7 @@
         <v>3</v>
       </c>
       <c r="B57" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C57">
         <v>255</v>
@@ -1253,7 +1253,7 @@
         <v>3</v>
       </c>
       <c r="B59" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C59">
         <v>274</v>
@@ -1281,7 +1281,7 @@
         <v>3</v>
       </c>
       <c r="B61" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61">
         <v>279</v>
@@ -1309,7 +1309,7 @@
         <v>3</v>
       </c>
       <c r="B63" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C63">
         <v>298</v>
@@ -1337,7 +1337,7 @@
         <v>3</v>
       </c>
       <c r="B65" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C65">
         <v>303</v>
@@ -1365,7 +1365,7 @@
         <v>3</v>
       </c>
       <c r="B67" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C67">
         <v>320</v>
@@ -1393,7 +1393,7 @@
         <v>4</v>
       </c>
       <c r="B69" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C69">
         <v>202</v>
@@ -1421,7 +1421,7 @@
         <v>4</v>
       </c>
       <c r="B71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C71">
         <v>209</v>
@@ -1449,7 +1449,7 @@
         <v>4</v>
       </c>
       <c r="B73" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C73">
         <v>226</v>
@@ -1477,7 +1477,7 @@
         <v>4</v>
       </c>
       <c r="B75" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75">
         <v>231</v>
@@ -1505,7 +1505,7 @@
         <v>4</v>
       </c>
       <c r="B77" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C77">
         <v>250</v>
@@ -1533,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="B79" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C79">
         <v>255</v>
@@ -1561,7 +1561,7 @@
         <v>4</v>
       </c>
       <c r="B81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C81">
         <v>274</v>
@@ -1589,7 +1589,7 @@
         <v>4</v>
       </c>
       <c r="B83" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C83">
         <v>279</v>
@@ -1617,7 +1617,7 @@
         <v>4</v>
       </c>
       <c r="B85" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C85">
         <v>298</v>
@@ -1645,7 +1645,7 @@
         <v>4</v>
       </c>
       <c r="B87" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C87">
         <v>303</v>
@@ -1673,7 +1673,7 @@
         <v>4</v>
       </c>
       <c r="B89" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89">
         <v>320</v>
@@ -1701,7 +1701,7 @@
         <v>5</v>
       </c>
       <c r="B91" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C91">
         <v>202</v>
@@ -1729,7 +1729,7 @@
         <v>5</v>
       </c>
       <c r="B93" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C93">
         <v>209</v>
@@ -1757,7 +1757,7 @@
         <v>5</v>
       </c>
       <c r="B95" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95">
         <v>226</v>
@@ -1785,7 +1785,7 @@
         <v>5</v>
       </c>
       <c r="B97" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C97">
         <v>231</v>
@@ -1813,7 +1813,7 @@
         <v>5</v>
       </c>
       <c r="B99" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C99">
         <v>250</v>
@@ -1841,7 +1841,7 @@
         <v>5</v>
       </c>
       <c r="B101" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C101">
         <v>255</v>
@@ -1869,7 +1869,7 @@
         <v>5</v>
       </c>
       <c r="B103" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C103">
         <v>274</v>
@@ -1897,7 +1897,7 @@
         <v>5</v>
       </c>
       <c r="B105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C105">
         <v>279</v>
@@ -1925,7 +1925,7 @@
         <v>5</v>
       </c>
       <c r="B107" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C107">
         <v>298</v>
@@ -1953,7 +1953,7 @@
         <v>5</v>
       </c>
       <c r="B109" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C109">
         <v>303</v>
@@ -1981,7 +1981,7 @@
         <v>5</v>
       </c>
       <c r="B111" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C111">
         <v>320</v>
@@ -2009,7 +2009,7 @@
         <v>6</v>
       </c>
       <c r="B113" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C113">
         <v>202</v>
@@ -2037,7 +2037,7 @@
         <v>6</v>
       </c>
       <c r="B115" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C115">
         <v>209</v>
@@ -2065,7 +2065,7 @@
         <v>6</v>
       </c>
       <c r="B117" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C117">
         <v>226</v>
@@ -2093,7 +2093,7 @@
         <v>6</v>
       </c>
       <c r="B119" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C119">
         <v>231</v>
@@ -2121,7 +2121,7 @@
         <v>6</v>
       </c>
       <c r="B121" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C121">
         <v>250</v>
@@ -2149,7 +2149,7 @@
         <v>6</v>
       </c>
       <c r="B123" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C123">
         <v>255</v>
@@ -2177,7 +2177,7 @@
         <v>6</v>
       </c>
       <c r="B125" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C125">
         <v>274</v>
@@ -2205,7 +2205,7 @@
         <v>6</v>
       </c>
       <c r="B127" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C127">
         <v>279</v>
@@ -2233,7 +2233,7 @@
         <v>6</v>
       </c>
       <c r="B129" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C129">
         <v>298</v>
@@ -2261,7 +2261,7 @@
         <v>6</v>
       </c>
       <c r="B131" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C131">
         <v>303</v>
@@ -2289,7 +2289,7 @@
         <v>6</v>
       </c>
       <c r="B133" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C133">
         <v>320</v>
@@ -2317,7 +2317,7 @@
         <v>7</v>
       </c>
       <c r="B135" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C135">
         <v>202</v>
@@ -2345,7 +2345,7 @@
         <v>7</v>
       </c>
       <c r="B137" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C137">
         <v>209</v>
@@ -2373,7 +2373,7 @@
         <v>7</v>
       </c>
       <c r="B139" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C139">
         <v>226</v>
@@ -2401,7 +2401,7 @@
         <v>7</v>
       </c>
       <c r="B141" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C141">
         <v>231</v>
@@ -2429,7 +2429,7 @@
         <v>7</v>
       </c>
       <c r="B143" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C143">
         <v>250</v>
@@ -2457,7 +2457,7 @@
         <v>7</v>
       </c>
       <c r="B145" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C145">
         <v>255</v>
@@ -2485,7 +2485,7 @@
         <v>7</v>
       </c>
       <c r="B147" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C147">
         <v>274</v>
@@ -2513,7 +2513,7 @@
         <v>7</v>
       </c>
       <c r="B149" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C149">
         <v>279</v>
@@ -2541,7 +2541,7 @@
         <v>7</v>
       </c>
       <c r="B151" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C151">
         <v>298</v>
@@ -2569,7 +2569,7 @@
         <v>7</v>
       </c>
       <c r="B153" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C153">
         <v>303</v>
@@ -2597,7 +2597,7 @@
         <v>7</v>
       </c>
       <c r="B155" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C155">
         <v>320</v>
@@ -2625,7 +2625,7 @@
         <v>8</v>
       </c>
       <c r="B157" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C157">
         <v>202</v>
@@ -2653,7 +2653,7 @@
         <v>8</v>
       </c>
       <c r="B159" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C159">
         <v>209</v>
@@ -2681,7 +2681,7 @@
         <v>8</v>
       </c>
       <c r="B161" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C161">
         <v>226</v>
@@ -2709,7 +2709,7 @@
         <v>8</v>
       </c>
       <c r="B163" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C163">
         <v>231</v>
@@ -2737,7 +2737,7 @@
         <v>8</v>
       </c>
       <c r="B165" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C165">
         <v>250</v>
@@ -2765,7 +2765,7 @@
         <v>8</v>
       </c>
       <c r="B167" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C167">
         <v>255</v>
@@ -2793,7 +2793,7 @@
         <v>8</v>
       </c>
       <c r="B169" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C169">
         <v>274</v>
@@ -2821,7 +2821,7 @@
         <v>8</v>
       </c>
       <c r="B171" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C171">
         <v>279</v>
@@ -2849,7 +2849,7 @@
         <v>8</v>
       </c>
       <c r="B173" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C173">
         <v>298</v>
@@ -2877,7 +2877,7 @@
         <v>8</v>
       </c>
       <c r="B175" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C175">
         <v>303</v>
@@ -2905,7 +2905,7 @@
         <v>8</v>
       </c>
       <c r="B177" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C177">
         <v>320</v>
@@ -2933,7 +2933,7 @@
         <v>9</v>
       </c>
       <c r="B179" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C179">
         <v>202</v>
@@ -2961,7 +2961,7 @@
         <v>9</v>
       </c>
       <c r="B181" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C181">
         <v>209</v>
@@ -2989,7 +2989,7 @@
         <v>9</v>
       </c>
       <c r="B183" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C183">
         <v>226</v>
@@ -3017,7 +3017,7 @@
         <v>9</v>
       </c>
       <c r="B185" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C185">
         <v>231</v>
@@ -3045,7 +3045,7 @@
         <v>9</v>
       </c>
       <c r="B187" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C187">
         <v>250</v>
@@ -3073,7 +3073,7 @@
         <v>9</v>
       </c>
       <c r="B189" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C189">
         <v>255</v>
@@ -3101,7 +3101,7 @@
         <v>9</v>
       </c>
       <c r="B191" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C191">
         <v>274</v>
@@ -3129,7 +3129,7 @@
         <v>9</v>
       </c>
       <c r="B193" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C193">
         <v>279</v>
@@ -3157,7 +3157,7 @@
         <v>9</v>
       </c>
       <c r="B195" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C195">
         <v>298</v>
@@ -3185,7 +3185,7 @@
         <v>9</v>
       </c>
       <c r="B197" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C197">
         <v>303</v>
@@ -3213,7 +3213,7 @@
         <v>9</v>
       </c>
       <c r="B199" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C199">
         <v>320</v>
@@ -3241,7 +3241,7 @@
         <v>10</v>
       </c>
       <c r="B201" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C201">
         <v>202</v>
@@ -3269,7 +3269,7 @@
         <v>10</v>
       </c>
       <c r="B203" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C203">
         <v>209</v>
@@ -3297,7 +3297,7 @@
         <v>10</v>
       </c>
       <c r="B205" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C205">
         <v>226</v>
@@ -3325,7 +3325,7 @@
         <v>10</v>
       </c>
       <c r="B207" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C207">
         <v>231</v>
@@ -3353,7 +3353,7 @@
         <v>10</v>
       </c>
       <c r="B209" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C209">
         <v>250</v>
@@ -3381,7 +3381,7 @@
         <v>10</v>
       </c>
       <c r="B211" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C211">
         <v>255</v>
@@ -3409,7 +3409,7 @@
         <v>10</v>
       </c>
       <c r="B213" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C213">
         <v>274</v>
@@ -3437,7 +3437,7 @@
         <v>10</v>
       </c>
       <c r="B215" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C215">
         <v>279</v>
@@ -3465,7 +3465,7 @@
         <v>10</v>
       </c>
       <c r="B217" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C217">
         <v>298</v>
@@ -3493,7 +3493,7 @@
         <v>10</v>
       </c>
       <c r="B219" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C219">
         <v>303</v>
@@ -3521,7 +3521,7 @@
         <v>10</v>
       </c>
       <c r="B221" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C221">
         <v>320</v>
@@ -3549,7 +3549,7 @@
         <v>11</v>
       </c>
       <c r="B223" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C223">
         <v>202</v>
@@ -3574,7 +3574,7 @@
         <v>11</v>
       </c>
       <c r="B225" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C225">
         <v>209</v>
@@ -3599,7 +3599,7 @@
         <v>11</v>
       </c>
       <c r="B227" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C227">
         <v>226</v>
@@ -3624,7 +3624,7 @@
         <v>11</v>
       </c>
       <c r="B229" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C229">
         <v>231</v>
@@ -3649,7 +3649,7 @@
         <v>11</v>
       </c>
       <c r="B231" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C231">
         <v>250</v>
@@ -3674,7 +3674,7 @@
         <v>11</v>
       </c>
       <c r="B233" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C233">
         <v>255</v>
@@ -3699,7 +3699,7 @@
         <v>11</v>
       </c>
       <c r="B235" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C235">
         <v>274</v>
@@ -3724,7 +3724,7 @@
         <v>11</v>
       </c>
       <c r="B237" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C237">
         <v>279</v>
@@ -3749,7 +3749,7 @@
         <v>11</v>
       </c>
       <c r="B239" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C239">
         <v>298</v>
@@ -3774,7 +3774,7 @@
         <v>11</v>
       </c>
       <c r="B241" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C241">
         <v>303</v>
@@ -3799,7 +3799,7 @@
         <v>11</v>
       </c>
       <c r="B243" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C243">
         <v>320</v>
@@ -3824,7 +3824,7 @@
         <v>12</v>
       </c>
       <c r="B245" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C245">
         <v>202</v>
@@ -3849,7 +3849,7 @@
         <v>12</v>
       </c>
       <c r="B247" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C247">
         <v>209</v>
@@ -3874,7 +3874,7 @@
         <v>12</v>
       </c>
       <c r="B249" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C249">
         <v>226</v>
@@ -3899,7 +3899,7 @@
         <v>12</v>
       </c>
       <c r="B251" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C251">
         <v>231</v>
@@ -3924,7 +3924,7 @@
         <v>12</v>
       </c>
       <c r="B253" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C253">
         <v>250</v>
@@ -3949,7 +3949,7 @@
         <v>12</v>
       </c>
       <c r="B255" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C255">
         <v>255</v>
@@ -3974,7 +3974,7 @@
         <v>12</v>
       </c>
       <c r="B257" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C257">
         <v>274</v>
@@ -3999,7 +3999,7 @@
         <v>12</v>
       </c>
       <c r="B259" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C259">
         <v>279</v>
@@ -4024,7 +4024,7 @@
         <v>12</v>
       </c>
       <c r="B261" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C261">
         <v>298</v>
@@ -4049,7 +4049,7 @@
         <v>12</v>
       </c>
       <c r="B263" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C263">
         <v>303</v>
@@ -4074,7 +4074,7 @@
         <v>12</v>
       </c>
       <c r="B265" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C265">
         <v>320</v>
@@ -4099,7 +4099,7 @@
         <v>13</v>
       </c>
       <c r="B267" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C267">
         <v>202</v>
@@ -4124,7 +4124,7 @@
         <v>13</v>
       </c>
       <c r="B269" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C269">
         <v>209</v>
@@ -4149,7 +4149,7 @@
         <v>13</v>
       </c>
       <c r="B271" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C271">
         <v>226</v>
@@ -4174,7 +4174,7 @@
         <v>13</v>
       </c>
       <c r="B273" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C273">
         <v>231</v>
@@ -4199,7 +4199,7 @@
         <v>13</v>
       </c>
       <c r="B275" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C275">
         <v>250</v>
@@ -4224,7 +4224,7 @@
         <v>13</v>
       </c>
       <c r="B277" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C277">
         <v>255</v>
@@ -4249,7 +4249,7 @@
         <v>13</v>
       </c>
       <c r="B279" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C279">
         <v>274</v>
@@ -4274,7 +4274,7 @@
         <v>13</v>
       </c>
       <c r="B281" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C281">
         <v>279</v>
@@ -4299,7 +4299,7 @@
         <v>13</v>
       </c>
       <c r="B283" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C283">
         <v>298</v>
@@ -4324,7 +4324,7 @@
         <v>13</v>
       </c>
       <c r="B285" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C285">
         <v>303</v>
@@ -4349,7 +4349,7 @@
         <v>13</v>
       </c>
       <c r="B287" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C287">
         <v>320</v>
@@ -4374,7 +4374,7 @@
         <v>14</v>
       </c>
       <c r="B289" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C289">
         <v>202</v>
@@ -4399,7 +4399,7 @@
         <v>14</v>
       </c>
       <c r="B291" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C291">
         <v>209</v>
@@ -4424,7 +4424,7 @@
         <v>14</v>
       </c>
       <c r="B293" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C293">
         <v>226</v>
@@ -4449,7 +4449,7 @@
         <v>14</v>
       </c>
       <c r="B295" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C295">
         <v>231</v>
@@ -4474,7 +4474,7 @@
         <v>14</v>
       </c>
       <c r="B297" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C297">
         <v>250</v>
@@ -4499,7 +4499,7 @@
         <v>14</v>
       </c>
       <c r="B299" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C299">
         <v>255</v>
@@ -4524,7 +4524,7 @@
         <v>14</v>
       </c>
       <c r="B301" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C301">
         <v>274</v>
@@ -4549,7 +4549,7 @@
         <v>14</v>
       </c>
       <c r="B303" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C303">
         <v>279</v>
@@ -4574,7 +4574,7 @@
         <v>14</v>
       </c>
       <c r="B305" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C305">
         <v>298</v>
@@ -4599,7 +4599,7 @@
         <v>14</v>
       </c>
       <c r="B307" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C307">
         <v>303</v>
@@ -4624,7 +4624,7 @@
         <v>14</v>
       </c>
       <c r="B309" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C309">
         <v>320</v>
@@ -4649,7 +4649,7 @@
         <v>15</v>
       </c>
       <c r="B311" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C311">
         <v>202</v>
@@ -4674,7 +4674,7 @@
         <v>15</v>
       </c>
       <c r="B313" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C313">
         <v>209</v>
@@ -4699,7 +4699,7 @@
         <v>15</v>
       </c>
       <c r="B315" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C315">
         <v>226</v>
@@ -4724,7 +4724,7 @@
         <v>15</v>
       </c>
       <c r="B317" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C317">
         <v>231</v>
@@ -4749,7 +4749,7 @@
         <v>15</v>
       </c>
       <c r="B319" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C319">
         <v>250</v>
@@ -4774,7 +4774,7 @@
         <v>15</v>
       </c>
       <c r="B321" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C321">
         <v>255</v>
@@ -4799,7 +4799,7 @@
         <v>15</v>
       </c>
       <c r="B323" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C323">
         <v>274</v>
@@ -4824,7 +4824,7 @@
         <v>15</v>
       </c>
       <c r="B325" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C325">
         <v>279</v>
@@ -4849,7 +4849,7 @@
         <v>15</v>
       </c>
       <c r="B327" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C327">
         <v>298</v>
@@ -4874,7 +4874,7 @@
         <v>15</v>
       </c>
       <c r="B329" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C329">
         <v>303</v>
@@ -4899,7 +4899,7 @@
         <v>15</v>
       </c>
       <c r="B331" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C331">
         <v>320</v>
@@ -4924,7 +4924,7 @@
         <v>16</v>
       </c>
       <c r="B333" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C333">
         <v>202</v>
@@ -4952,7 +4952,7 @@
         <v>16</v>
       </c>
       <c r="B335" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C335">
         <v>209</v>
@@ -4980,7 +4980,7 @@
         <v>16</v>
       </c>
       <c r="B337" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C337">
         <v>226</v>
@@ -5008,7 +5008,7 @@
         <v>16</v>
       </c>
       <c r="B339" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C339">
         <v>231</v>
@@ -5036,7 +5036,7 @@
         <v>16</v>
       </c>
       <c r="B341" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C341">
         <v>250</v>
@@ -5064,7 +5064,7 @@
         <v>16</v>
       </c>
       <c r="B343" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C343">
         <v>255</v>
@@ -5092,7 +5092,7 @@
         <v>16</v>
       </c>
       <c r="B345" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C345">
         <v>274</v>
@@ -5120,7 +5120,7 @@
         <v>16</v>
       </c>
       <c r="B347" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C347">
         <v>279</v>
@@ -5148,7 +5148,7 @@
         <v>16</v>
       </c>
       <c r="B349" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C349">
         <v>298</v>
@@ -5176,7 +5176,7 @@
         <v>16</v>
       </c>
       <c r="B351" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C351">
         <v>303</v>
@@ -5204,7 +5204,7 @@
         <v>16</v>
       </c>
       <c r="B353" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C353">
         <v>320</v>
@@ -5232,7 +5232,7 @@
         <v>17</v>
       </c>
       <c r="B355" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C355">
         <v>202</v>
@@ -5260,7 +5260,7 @@
         <v>17</v>
       </c>
       <c r="B357" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C357">
         <v>209</v>
@@ -5288,7 +5288,7 @@
         <v>17</v>
       </c>
       <c r="B359" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C359">
         <v>226</v>
@@ -5316,7 +5316,7 @@
         <v>17</v>
       </c>
       <c r="B361" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C361">
         <v>231</v>
@@ -5344,7 +5344,7 @@
         <v>17</v>
       </c>
       <c r="B363" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C363">
         <v>250</v>
@@ -5372,7 +5372,7 @@
         <v>17</v>
       </c>
       <c r="B365" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C365">
         <v>255</v>
@@ -5400,7 +5400,7 @@
         <v>17</v>
       </c>
       <c r="B367" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C367">
         <v>274</v>
@@ -5428,7 +5428,7 @@
         <v>17</v>
       </c>
       <c r="B369" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C369">
         <v>279</v>
@@ -5456,7 +5456,7 @@
         <v>17</v>
       </c>
       <c r="B371" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C371">
         <v>298</v>
@@ -5484,7 +5484,7 @@
         <v>17</v>
       </c>
       <c r="B373" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C373">
         <v>303</v>
@@ -5512,7 +5512,7 @@
         <v>17</v>
       </c>
       <c r="B375" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C375">
         <v>320</v>
@@ -5540,7 +5540,7 @@
         <v>18</v>
       </c>
       <c r="B377" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C377">
         <v>202</v>
@@ -5568,7 +5568,7 @@
         <v>18</v>
       </c>
       <c r="B379" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C379">
         <v>209</v>
@@ -5596,7 +5596,7 @@
         <v>18</v>
       </c>
       <c r="B381" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C381">
         <v>226</v>
@@ -5624,7 +5624,7 @@
         <v>18</v>
       </c>
       <c r="B383" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C383">
         <v>231</v>
@@ -5652,7 +5652,7 @@
         <v>18</v>
       </c>
       <c r="B385" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C385">
         <v>250</v>
@@ -5680,7 +5680,7 @@
         <v>18</v>
       </c>
       <c r="B387" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C387">
         <v>255</v>
@@ -5708,7 +5708,7 @@
         <v>18</v>
       </c>
       <c r="B389" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C389">
         <v>274</v>
@@ -5736,7 +5736,7 @@
         <v>18</v>
       </c>
       <c r="B391" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C391">
         <v>279</v>
@@ -5764,7 +5764,7 @@
         <v>18</v>
       </c>
       <c r="B393" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C393">
         <v>298</v>
@@ -5792,7 +5792,7 @@
         <v>18</v>
       </c>
       <c r="B395" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C395">
         <v>303</v>
@@ -5820,7 +5820,7 @@
         <v>18</v>
       </c>
       <c r="B397" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C397">
         <v>320</v>
@@ -5848,7 +5848,7 @@
         <v>19</v>
       </c>
       <c r="B399" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C399">
         <v>202</v>
@@ -5876,7 +5876,7 @@
         <v>19</v>
       </c>
       <c r="B401" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C401">
         <v>209</v>
@@ -5904,7 +5904,7 @@
         <v>19</v>
       </c>
       <c r="B403" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C403">
         <v>226</v>
@@ -5932,7 +5932,7 @@
         <v>19</v>
       </c>
       <c r="B405" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C405">
         <v>231</v>
@@ -5960,7 +5960,7 @@
         <v>19</v>
       </c>
       <c r="B407" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C407">
         <v>250</v>
@@ -5988,7 +5988,7 @@
         <v>19</v>
       </c>
       <c r="B409" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C409">
         <v>255</v>
@@ -6016,7 +6016,7 @@
         <v>19</v>
       </c>
       <c r="B411" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C411">
         <v>274</v>
@@ -6044,7 +6044,7 @@
         <v>19</v>
       </c>
       <c r="B413" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C413">
         <v>279</v>
@@ -6072,7 +6072,7 @@
         <v>19</v>
       </c>
       <c r="B415" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C415">
         <v>298</v>
@@ -6100,7 +6100,7 @@
         <v>19</v>
       </c>
       <c r="B417" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C417">
         <v>303</v>
@@ -6128,7 +6128,7 @@
         <v>19</v>
       </c>
       <c r="B419" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C419">
         <v>320</v>
@@ -6156,7 +6156,7 @@
         <v>20</v>
       </c>
       <c r="B421" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C421">
         <v>202</v>
@@ -6184,7 +6184,7 @@
         <v>20</v>
       </c>
       <c r="B423" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C423">
         <v>209</v>
@@ -6212,7 +6212,7 @@
         <v>20</v>
       </c>
       <c r="B425" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C425">
         <v>226</v>
@@ -6240,7 +6240,7 @@
         <v>20</v>
       </c>
       <c r="B427" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C427">
         <v>231</v>
@@ -6268,7 +6268,7 @@
         <v>20</v>
       </c>
       <c r="B429" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C429">
         <v>250</v>
@@ -6296,7 +6296,7 @@
         <v>20</v>
       </c>
       <c r="B431" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C431">
         <v>255</v>
@@ -6324,7 +6324,7 @@
         <v>20</v>
       </c>
       <c r="B433" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C433">
         <v>274</v>
@@ -6352,7 +6352,7 @@
         <v>20</v>
       </c>
       <c r="B435" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C435">
         <v>279</v>
@@ -6380,7 +6380,7 @@
         <v>20</v>
       </c>
       <c r="B437" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C437">
         <v>298</v>
@@ -6408,7 +6408,7 @@
         <v>20</v>
       </c>
       <c r="B439" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C439">
         <v>303</v>
@@ -6436,7 +6436,7 @@
         <v>20</v>
       </c>
       <c r="B441" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C441">
         <v>320</v>
@@ -6464,7 +6464,7 @@
         <v>21</v>
       </c>
       <c r="B443" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C443">
         <v>202</v>
@@ -6492,7 +6492,7 @@
         <v>21</v>
       </c>
       <c r="B445" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C445">
         <v>209</v>
@@ -6520,7 +6520,7 @@
         <v>21</v>
       </c>
       <c r="B447" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C447">
         <v>226</v>
@@ -6548,7 +6548,7 @@
         <v>21</v>
       </c>
       <c r="B449" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C449">
         <v>231</v>
@@ -6576,7 +6576,7 @@
         <v>21</v>
       </c>
       <c r="B451" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C451">
         <v>250</v>
@@ -6604,7 +6604,7 @@
         <v>21</v>
       </c>
       <c r="B453" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C453">
         <v>255</v>
@@ -6632,7 +6632,7 @@
         <v>21</v>
       </c>
       <c r="B455" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C455">
         <v>274</v>
@@ -6660,7 +6660,7 @@
         <v>21</v>
       </c>
       <c r="B457" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C457">
         <v>279</v>
@@ -6688,7 +6688,7 @@
         <v>21</v>
       </c>
       <c r="B459" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C459">
         <v>298</v>
@@ -6716,7 +6716,7 @@
         <v>21</v>
       </c>
       <c r="B461" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C461">
         <v>303</v>
@@ -6744,7 +6744,7 @@
         <v>21</v>
       </c>
       <c r="B463" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C463">
         <v>320</v>
@@ -6772,7 +6772,7 @@
         <v>22</v>
       </c>
       <c r="B465" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C465">
         <v>202</v>
@@ -6800,7 +6800,7 @@
         <v>22</v>
       </c>
       <c r="B467" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C467">
         <v>209</v>
@@ -6828,7 +6828,7 @@
         <v>22</v>
       </c>
       <c r="B469" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C469">
         <v>226</v>
@@ -6856,7 +6856,7 @@
         <v>22</v>
       </c>
       <c r="B471" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C471">
         <v>231</v>
@@ -6884,7 +6884,7 @@
         <v>22</v>
       </c>
       <c r="B473" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C473">
         <v>250</v>
@@ -6912,7 +6912,7 @@
         <v>22</v>
       </c>
       <c r="B475" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C475">
         <v>255</v>
@@ -6940,7 +6940,7 @@
         <v>22</v>
       </c>
       <c r="B477" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C477">
         <v>274</v>
@@ -6968,7 +6968,7 @@
         <v>22</v>
       </c>
       <c r="B479" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C479">
         <v>279</v>
@@ -6996,7 +6996,7 @@
         <v>22</v>
       </c>
       <c r="B481" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C481">
         <v>298</v>
@@ -7024,7 +7024,7 @@
         <v>22</v>
       </c>
       <c r="B483" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C483">
         <v>303</v>
@@ -7052,7 +7052,7 @@
         <v>22</v>
       </c>
       <c r="B485" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C485">
         <v>320</v>
@@ -7080,7 +7080,7 @@
         <v>23</v>
       </c>
       <c r="B487" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C487">
         <v>202</v>
@@ -7108,7 +7108,7 @@
         <v>23</v>
       </c>
       <c r="B489" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C489">
         <v>209</v>
@@ -7136,7 +7136,7 @@
         <v>23</v>
       </c>
       <c r="B491" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C491">
         <v>226</v>
@@ -7164,7 +7164,7 @@
         <v>23</v>
       </c>
       <c r="B493" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C493">
         <v>231</v>
@@ -7192,7 +7192,7 @@
         <v>23</v>
       </c>
       <c r="B495" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C495">
         <v>250</v>
@@ -7220,7 +7220,7 @@
         <v>23</v>
       </c>
       <c r="B497" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C497">
         <v>255</v>
@@ -7248,7 +7248,7 @@
         <v>23</v>
       </c>
       <c r="B499" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C499">
         <v>274</v>
@@ -7276,7 +7276,7 @@
         <v>23</v>
       </c>
       <c r="B501" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C501">
         <v>279</v>
@@ -7304,7 +7304,7 @@
         <v>23</v>
       </c>
       <c r="B503" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C503">
         <v>298</v>
@@ -7332,7 +7332,7 @@
         <v>23</v>
       </c>
       <c r="B505" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C505">
         <v>303</v>
@@ -7360,7 +7360,7 @@
         <v>23</v>
       </c>
       <c r="B507" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C507">
         <v>320</v>
@@ -7388,7 +7388,7 @@
         <v>24</v>
       </c>
       <c r="B509" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C509">
         <v>202</v>
@@ -7416,7 +7416,7 @@
         <v>24</v>
       </c>
       <c r="B511" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C511">
         <v>209</v>
@@ -7444,7 +7444,7 @@
         <v>24</v>
       </c>
       <c r="B513" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C513">
         <v>226</v>
@@ -7472,7 +7472,7 @@
         <v>24</v>
       </c>
       <c r="B515" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C515">
         <v>231</v>
@@ -7500,7 +7500,7 @@
         <v>24</v>
       </c>
       <c r="B517" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C517">
         <v>250</v>
@@ -7528,7 +7528,7 @@
         <v>24</v>
       </c>
       <c r="B519" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C519">
         <v>255</v>
@@ -7556,7 +7556,7 @@
         <v>24</v>
       </c>
       <c r="B521" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C521">
         <v>274</v>
@@ -7584,7 +7584,7 @@
         <v>24</v>
       </c>
       <c r="B523" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C523">
         <v>279</v>
@@ -7612,7 +7612,7 @@
         <v>24</v>
       </c>
       <c r="B525" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C525">
         <v>298</v>
@@ -7640,7 +7640,7 @@
         <v>24</v>
       </c>
       <c r="B527" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C527">
         <v>303</v>
@@ -7668,7 +7668,7 @@
         <v>24</v>
       </c>
       <c r="B529" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C529">
         <v>320</v>
@@ -7696,7 +7696,7 @@
         <v>25</v>
       </c>
       <c r="B531" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C531">
         <v>202</v>
@@ -7724,7 +7724,7 @@
         <v>25</v>
       </c>
       <c r="B533" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C533">
         <v>209</v>
@@ -7752,7 +7752,7 @@
         <v>25</v>
       </c>
       <c r="B535" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C535">
         <v>226</v>
@@ -7780,7 +7780,7 @@
         <v>25</v>
       </c>
       <c r="B537" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C537">
         <v>231</v>
@@ -7808,7 +7808,7 @@
         <v>25</v>
       </c>
       <c r="B539" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C539">
         <v>250</v>
@@ -7836,7 +7836,7 @@
         <v>25</v>
       </c>
       <c r="B541" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C541">
         <v>255</v>
@@ -7864,7 +7864,7 @@
         <v>25</v>
       </c>
       <c r="B543" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C543">
         <v>274</v>
@@ -7892,7 +7892,7 @@
         <v>25</v>
       </c>
       <c r="B545" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C545">
         <v>279</v>
@@ -7920,7 +7920,7 @@
         <v>25</v>
       </c>
       <c r="B547" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C547">
         <v>298</v>
@@ -7948,7 +7948,7 @@
         <v>25</v>
       </c>
       <c r="B549" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C549">
         <v>303</v>
@@ -7976,7 +7976,7 @@
         <v>25</v>
       </c>
       <c r="B551" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C551">
         <v>320</v>
@@ -8004,7 +8004,7 @@
         <v>26</v>
       </c>
       <c r="B553" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C553">
         <v>202</v>
@@ -8032,7 +8032,7 @@
         <v>26</v>
       </c>
       <c r="B555" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C555">
         <v>209</v>
@@ -8060,7 +8060,7 @@
         <v>26</v>
       </c>
       <c r="B557" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C557">
         <v>226</v>
@@ -8088,7 +8088,7 @@
         <v>26</v>
       </c>
       <c r="B559" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C559">
         <v>231</v>
@@ -8116,7 +8116,7 @@
         <v>26</v>
       </c>
       <c r="B561" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C561">
         <v>250</v>
@@ -8144,7 +8144,7 @@
         <v>26</v>
       </c>
       <c r="B563" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C563">
         <v>255</v>
@@ -8172,7 +8172,7 @@
         <v>26</v>
       </c>
       <c r="B565" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C565">
         <v>274</v>
@@ -8200,7 +8200,7 @@
         <v>26</v>
       </c>
       <c r="B567" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C567">
         <v>279</v>
@@ -8228,7 +8228,7 @@
         <v>26</v>
       </c>
       <c r="B569" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C569">
         <v>298</v>
@@ -8256,7 +8256,7 @@
         <v>26</v>
       </c>
       <c r="B571" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C571">
         <v>303</v>
@@ -8284,7 +8284,7 @@
         <v>26</v>
       </c>
       <c r="B573" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C573">
         <v>320</v>
@@ -8312,7 +8312,7 @@
         <v>27</v>
       </c>
       <c r="B575" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C575">
         <v>202</v>
@@ -8340,7 +8340,7 @@
         <v>27</v>
       </c>
       <c r="B577" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C577">
         <v>209</v>
@@ -8368,7 +8368,7 @@
         <v>27</v>
       </c>
       <c r="B579" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C579">
         <v>226</v>
@@ -8396,7 +8396,7 @@
         <v>27</v>
       </c>
       <c r="B581" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C581">
         <v>231</v>
@@ -8424,7 +8424,7 @@
         <v>27</v>
       </c>
       <c r="B583" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C583">
         <v>250</v>
@@ -8452,7 +8452,7 @@
         <v>27</v>
       </c>
       <c r="B585" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C585">
         <v>255</v>
@@ -8480,7 +8480,7 @@
         <v>27</v>
       </c>
       <c r="B587" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C587">
         <v>274</v>
@@ -8508,7 +8508,7 @@
         <v>27</v>
       </c>
       <c r="B589" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C589">
         <v>279</v>
@@ -8536,7 +8536,7 @@
         <v>27</v>
       </c>
       <c r="B591" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C591">
         <v>298</v>
@@ -8564,7 +8564,7 @@
         <v>27</v>
       </c>
       <c r="B593" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C593">
         <v>303</v>
@@ -8592,7 +8592,7 @@
         <v>27</v>
       </c>
       <c r="B595" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C595">
         <v>320</v>
@@ -8620,7 +8620,7 @@
         <v>28</v>
       </c>
       <c r="B597" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C597">
         <v>202</v>
@@ -8648,7 +8648,7 @@
         <v>28</v>
       </c>
       <c r="B599" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C599">
         <v>209</v>
@@ -8676,7 +8676,7 @@
         <v>28</v>
       </c>
       <c r="B601" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C601">
         <v>226</v>
@@ -8704,7 +8704,7 @@
         <v>28</v>
       </c>
       <c r="B603" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C603">
         <v>231</v>
@@ -8732,7 +8732,7 @@
         <v>28</v>
       </c>
       <c r="B605" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C605">
         <v>250</v>
@@ -8760,7 +8760,7 @@
         <v>28</v>
       </c>
       <c r="B607" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C607">
         <v>255</v>
@@ -8788,7 +8788,7 @@
         <v>28</v>
       </c>
       <c r="B609" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C609">
         <v>274</v>
@@ -8816,7 +8816,7 @@
         <v>28</v>
       </c>
       <c r="B611" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C611">
         <v>279</v>
@@ -8844,7 +8844,7 @@
         <v>28</v>
       </c>
       <c r="B613" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C613">
         <v>298</v>
@@ -8872,7 +8872,7 @@
         <v>28</v>
       </c>
       <c r="B615" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C615">
         <v>303</v>
@@ -8900,7 +8900,7 @@
         <v>28</v>
       </c>
       <c r="B617" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C617">
         <v>320</v>
@@ -8928,7 +8928,7 @@
         <v>29</v>
       </c>
       <c r="B619" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C619">
         <v>202</v>
@@ -8956,7 +8956,7 @@
         <v>29</v>
       </c>
       <c r="B621" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C621">
         <v>209</v>
@@ -8984,7 +8984,7 @@
         <v>29</v>
       </c>
       <c r="B623" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C623">
         <v>226</v>
@@ -9012,7 +9012,7 @@
         <v>29</v>
       </c>
       <c r="B625" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C625">
         <v>231</v>
@@ -9040,7 +9040,7 @@
         <v>29</v>
       </c>
       <c r="B627" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C627">
         <v>250</v>
@@ -9068,7 +9068,7 @@
         <v>29</v>
       </c>
       <c r="B629" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C629">
         <v>255</v>
@@ -9096,7 +9096,7 @@
         <v>29</v>
       </c>
       <c r="B631" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C631">
         <v>274</v>
@@ -9124,7 +9124,7 @@
         <v>29</v>
       </c>
       <c r="B633" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C633">
         <v>279</v>
@@ -9152,7 +9152,7 @@
         <v>29</v>
       </c>
       <c r="B635" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C635">
         <v>298</v>
@@ -9180,7 +9180,7 @@
         <v>29</v>
       </c>
       <c r="B637" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C637">
         <v>303</v>
@@ -9208,7 +9208,7 @@
         <v>29</v>
       </c>
       <c r="B639" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C639">
         <v>320</v>
@@ -9236,7 +9236,7 @@
         <v>30</v>
       </c>
       <c r="B641" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C641">
         <v>202</v>
@@ -9264,7 +9264,7 @@
         <v>30</v>
       </c>
       <c r="B643" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C643">
         <v>209</v>
@@ -9292,7 +9292,7 @@
         <v>30</v>
       </c>
       <c r="B645" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C645">
         <v>226</v>
@@ -9320,7 +9320,7 @@
         <v>30</v>
       </c>
       <c r="B647" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C647">
         <v>231</v>
@@ -9348,7 +9348,7 @@
         <v>30</v>
       </c>
       <c r="B649" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C649">
         <v>250</v>
@@ -9376,7 +9376,7 @@
         <v>30</v>
       </c>
       <c r="B651" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C651">
         <v>255</v>
@@ -9404,7 +9404,7 @@
         <v>30</v>
       </c>
       <c r="B653" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C653">
         <v>274</v>
@@ -9432,7 +9432,7 @@
         <v>30</v>
       </c>
       <c r="B655" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C655">
         <v>279</v>
@@ -9460,7 +9460,7 @@
         <v>30</v>
       </c>
       <c r="B657" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C657">
         <v>298</v>
@@ -9488,7 +9488,7 @@
         <v>30</v>
       </c>
       <c r="B659" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C659">
         <v>303</v>
@@ -9516,7 +9516,7 @@
         <v>30</v>
       </c>
       <c r="B661" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C661">
         <v>320</v>

</xml_diff>